<commit_message>
Feat: Added more meta data read out (mainly numbers) to OD
</commit_message>
<xml_diff>
--- a/data_analysis/OD_measurements_example.xlsx
+++ b/data_analysis/OD_measurements_example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Timon\notes\OD_measurement_16_5_23\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\timon\source\repos\my_stuff\data_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB062D9A-E1AD-4FE9-B86F-82B0C55E4C08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{373607E7-2CD3-411C-A271-3D6DD4FE9BF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6000" yWindow="6045" windowWidth="21015" windowHeight="8910" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21156" yWindow="5820" windowWidth="22896" windowHeight="13992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>MMY118-2c</t>
   </si>
@@ -44,13 +44,30 @@
   <si>
     <t>ASY076-1</t>
   </si>
+  <si>
+    <t>Timepoints</t>
+  </si>
+  <si>
+    <t>Horm. Conc.</t>
+  </si>
+  <si>
+    <t>Culture</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -66,7 +83,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -74,14 +91,112 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -362,614 +477,649 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:I26"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:H15"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C2" s="1">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="4"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B2" s="2"/>
+      <c r="C2" s="7">
         <v>0.46180555555555558</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="7">
         <v>0.51041666666666663</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="7">
         <v>0.55694444444444446</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="7">
         <v>0.59513888888888888</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" s="7">
         <v>0.63263888888888886</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2" s="7">
         <v>0.67152777777777783</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>0</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="8">
         <v>0.08</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="8">
         <v>0.09</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="8">
         <v>0.11</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="8">
         <v>0.14000000000000001</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="8">
         <v>0.19</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="8">
         <v>0.22</v>
       </c>
-      <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B4">
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="10"/>
+      <c r="B4" s="2">
         <v>5</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="8">
         <v>0.14000000000000001</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="8">
         <v>0.18</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="8">
         <v>0.23</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="8">
         <v>0.28999999999999998</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="8">
         <v>0.37</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="8">
         <v>0.46</v>
       </c>
-      <c r="I4" s="2"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B5">
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="10"/>
+      <c r="B5" s="2">
         <v>50</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="8">
         <v>0.14000000000000001</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="8">
         <v>0.18</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="8">
         <v>0.24</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="8">
         <v>0.28000000000000003</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="8">
         <v>0.4</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="8">
         <v>0.49</v>
       </c>
-      <c r="I5" s="2"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B6">
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="11"/>
+      <c r="B6" s="2">
         <v>100</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="8">
         <v>0.12</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="8">
         <v>0.15</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="8">
         <v>0.2</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="8">
         <v>0.25</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="8">
         <v>0.32</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="8">
         <v>0.39</v>
       </c>
-      <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="2">
         <v>0</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="8">
         <v>0.13</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="8">
         <v>0.16</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="8">
         <v>0.21</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="8">
         <v>0.28000000000000003</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="8">
         <v>0.32</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="8">
         <v>0.4</v>
       </c>
-      <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B8">
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="10"/>
+      <c r="B8" s="2">
         <v>5</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="8">
         <v>0.17</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="8">
         <v>0.21</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="8">
         <v>0.26</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="8">
         <v>0.28999999999999998</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="8">
         <v>0.36</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="8">
         <v>0.45</v>
       </c>
-      <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B9">
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="10"/>
+      <c r="B9" s="2">
         <v>50</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="8">
         <v>0.11</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="8">
         <v>0.13</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="8">
         <v>0.15</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="8">
         <v>0.15</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="8">
         <v>0.17</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="8">
         <v>0.21</v>
       </c>
-      <c r="I9" s="2"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B10">
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="11"/>
+      <c r="B10" s="2">
         <v>100</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="8">
         <v>0.22</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="8">
         <v>0.22</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="8">
         <v>0.27</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="8">
         <v>0.26</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="8">
         <v>0.28000000000000003</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10" s="8">
         <v>0.35</v>
       </c>
-      <c r="I10" s="2"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="2">
         <v>0</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="8">
         <v>0.09</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="8">
         <v>0.11</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="8">
         <v>0.14000000000000001</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="8">
         <v>0.16</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11" s="8">
         <v>0.21</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H11" s="8">
         <v>0.26</v>
       </c>
-      <c r="I11" s="2"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B12">
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="10"/>
+      <c r="B12" s="2">
         <v>5</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="8">
         <v>0.11</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="8">
         <v>0.14000000000000001</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="8">
         <v>0.18</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="8">
         <v>0.2</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12" s="8">
         <v>0.27</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12" s="8">
         <v>0.31</v>
       </c>
-      <c r="I12" s="2"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B13">
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="10"/>
+      <c r="B13" s="2">
         <v>50</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="8">
         <v>0.1</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="8">
         <v>0.13</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="8">
         <v>0.15</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="8">
         <v>0.14000000000000001</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13" s="8">
         <v>0.19</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H13" s="8">
         <v>0.2</v>
       </c>
-      <c r="I13" s="2"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B14">
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="11"/>
+      <c r="B14" s="2">
         <v>100</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="8">
         <v>0.41</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="8">
         <v>0.41</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="8">
         <v>0.48</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="8">
         <v>0.47</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G14" s="8">
         <v>0.57999999999999996</v>
       </c>
-      <c r="H14" s="2">
+      <c r="H14" s="8">
         <v>0.65</v>
       </c>
-      <c r="I14" s="2"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="2">
         <v>0</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="8">
         <v>0.13</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="8">
         <v>0.25</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="8">
         <v>0.28000000000000003</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="8">
         <v>0.34</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15" s="8">
         <v>0.44</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H15" s="8">
         <v>0.52</v>
       </c>
-      <c r="I15" s="2"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B16">
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="10"/>
+      <c r="B16" s="2">
         <v>5</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="8">
         <v>0.12</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="8">
         <v>0.12</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="8">
         <v>0.18</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="8">
         <v>0.22</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G16" s="8">
         <v>0.28000000000000003</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H16" s="8">
         <v>0.34</v>
       </c>
-      <c r="I16" s="2"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B17">
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="10"/>
+      <c r="B17" s="2">
         <v>50</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="8">
         <v>0.08</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="8">
         <v>0.17</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="8">
         <v>0.21</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17" s="8">
         <v>0.22</v>
       </c>
-      <c r="G17" s="2">
+      <c r="G17" s="8">
         <v>0.27</v>
       </c>
-      <c r="H17" s="2">
+      <c r="H17" s="8">
         <v>0.31</v>
       </c>
-      <c r="I17" s="2"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B18">
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="11"/>
+      <c r="B18" s="2">
         <v>100</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="8">
         <v>0.08</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="8">
         <v>0.23</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="8">
         <v>0.26</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="8">
         <v>0.28999999999999998</v>
       </c>
-      <c r="G18" s="2">
+      <c r="G18" s="8">
         <v>0.32</v>
       </c>
-      <c r="H18" s="2">
+      <c r="H18" s="8">
         <v>0.36</v>
       </c>
-      <c r="I18" s="2"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="2">
         <v>0</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="8">
         <v>0.08</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="8">
         <v>0.09</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19" s="8">
         <v>0.09</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F19" s="8">
         <v>0.11</v>
       </c>
-      <c r="G19" s="2">
+      <c r="G19" s="8">
         <v>0.12</v>
       </c>
-      <c r="H19" s="2">
+      <c r="H19" s="8">
         <v>0.14000000000000001</v>
       </c>
-      <c r="I19" s="2"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B20">
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="10"/>
+      <c r="B20" s="2">
         <v>5</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="8">
         <v>0.08</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="8">
         <v>0.11</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="8">
         <v>0.15</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20" s="8">
         <v>0.14000000000000001</v>
       </c>
-      <c r="G20" s="2">
+      <c r="G20" s="8">
         <v>0.16</v>
       </c>
-      <c r="H20" s="2">
+      <c r="H20" s="8">
         <v>0.17</v>
       </c>
-      <c r="I20" s="2"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B21">
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="10"/>
+      <c r="B21" s="2">
         <v>50</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="8">
         <v>0.11</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21" s="8">
         <v>0.13</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21" s="8">
         <v>0.12</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F21" s="8">
         <v>0.15</v>
       </c>
-      <c r="G21" s="2">
+      <c r="G21" s="8">
         <v>0.16</v>
       </c>
-      <c r="H21" s="2">
+      <c r="H21" s="8">
         <v>0.16</v>
       </c>
-      <c r="I21" s="2"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B22">
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="11"/>
+      <c r="B22" s="2">
         <v>100</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="8">
         <v>0.08</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22" s="8">
         <v>0.08</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22" s="8">
         <v>0.11</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F22" s="8">
         <v>0.09</v>
       </c>
-      <c r="G22" s="2">
+      <c r="G22" s="8">
         <v>0.09</v>
       </c>
-      <c r="H22" s="2">
+      <c r="H22" s="8">
         <v>0.1</v>
       </c>
-      <c r="I22" s="2"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="2">
         <v>0</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="8">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23" s="8">
         <v>0.08</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23" s="8">
         <v>0.06</v>
       </c>
-      <c r="F23" s="2">
+      <c r="F23" s="8">
         <v>0.1</v>
       </c>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B24">
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="10"/>
+      <c r="B24" s="2">
         <v>5</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="8">
         <v>0.05</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D24" s="8">
         <v>0.06</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E24" s="8">
         <v>0.08</v>
       </c>
-      <c r="F24" s="2">
+      <c r="F24" s="8">
         <v>0.08</v>
       </c>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B25">
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="1"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="10"/>
+      <c r="B25" s="2">
         <v>50</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="8">
         <v>0.06</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D25" s="8">
         <v>0.08</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E25" s="8">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="F25" s="2">
+      <c r="F25" s="8">
         <v>0.1</v>
       </c>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B26">
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="1"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="11"/>
+      <c r="B26" s="2">
         <v>100</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26" s="8">
         <v>0.05</v>
       </c>
-      <c r="D26" s="2">
+      <c r="D26" s="8">
         <v>0.06</v>
       </c>
-      <c r="E26" s="2">
+      <c r="E26" s="8">
         <v>0.09</v>
       </c>
-      <c r="F26" s="2">
+      <c r="F26" s="8">
         <v>0.06</v>
       </c>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>